<commit_message>
more audio + try recording
</commit_message>
<xml_diff>
--- a/new_bci_framework/paradigm/p300_paradigm/stim_words.xlsx
+++ b/new_bci_framework/paradigm/p300_paradigm/stim_words.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Toolboxes\GitHub\BCI4ALS-MI\python\bci4als-2022-python\new_bci_framework\paradigm\p300_paradigm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BE2EFD-3408-4FAE-BEF4-6EAE056FAA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C53A7ED-C95B-4D0A-A56B-3B4B72A36109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4170" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -143,12 +143,64 @@
         </r>
       </text>
     </comment>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{F81BBBE8-FE2C-463F-85E9-1C430E55C8F1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">Values
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>Each iteration of this loop, a different one of these values will be chosen. This will be the value of the variable named above.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{288AE536-1EA8-49D0-BBE5-1830332191F0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">Values
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>Each iteration of this loop, a different one of these values will be chosen. This will be the value of the variable named above.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="28">
   <si>
     <t>word</t>
   </si>
@@ -156,6 +208,12 @@
     <t>color</t>
   </si>
   <si>
+    <t>ןכ</t>
+  </si>
+  <si>
+    <t>אל</t>
+  </si>
+  <si>
     <t>black</t>
   </si>
   <si>
@@ -177,22 +235,55 @@
     <t>sound_target</t>
   </si>
   <si>
-    <t>כן</t>
-  </si>
-  <si>
-    <t>לא</t>
-  </si>
-  <si>
-    <t>רעש</t>
-  </si>
-  <si>
-    <t>YEShebYardenSHORT.wav</t>
-  </si>
-  <si>
-    <t>NOhebYardenSHORT.wav</t>
-  </si>
-  <si>
-    <t>PinkNoise.wav</t>
+    <t>שער</t>
+  </si>
+  <si>
+    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\NOhebYardenSHORT.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\YEShebYardenSHORT.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\PinkNoise.wav</t>
+  </si>
+  <si>
+    <t>came</t>
+  </si>
+  <si>
+    <t>hot</t>
+  </si>
+  <si>
+    <t>indicator</t>
+  </si>
+  <si>
+    <t>candle</t>
+  </si>
+  <si>
+    <t>רנ</t>
+  </si>
+  <si>
+    <t>דמ</t>
+  </si>
+  <si>
+    <t>םח</t>
+  </si>
+  <si>
+    <t>אב</t>
+  </si>
+  <si>
+    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\CAMEhebYarden.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\CANDLEhebYarden.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\HOThebYarden.wav</t>
+  </si>
+  <si>
+    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\INDICATORhebYarden.wav</t>
+  </si>
+  <si>
+    <t>target</t>
   </si>
 </sst>
 </file>
@@ -587,22 +678,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1"/>
-    <col min="4" max="16384" width="20.7109375" style="2"/>
+    <col min="4" max="4" width="64.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="20.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -611,49 +703,282 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -783,18 +1108,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -814,14 +1139,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -834,4 +1151,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix audio file paths
</commit_message>
<xml_diff>
--- a/new_bci_framework/paradigm/p300_paradigm/stim_words.xlsx
+++ b/new_bci_framework/paradigm/p300_paradigm/stim_words.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Toolboxes\GitHub\BCI4ALS-MI\python\bci4als-2022-python\new_bci_framework\paradigm\p300_paradigm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C53A7ED-C95B-4D0A-A56B-3B4B72A36109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64667C0-17AC-4644-A19B-3C3ED6A39F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,15 +238,6 @@
     <t>שער</t>
   </si>
   <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\NOhebYardenSHORT.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\YEShebYardenSHORT.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\PinkNoise.wav</t>
-  </si>
-  <si>
     <t>came</t>
   </si>
   <si>
@@ -271,19 +262,28 @@
     <t>אב</t>
   </si>
   <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\CAMEhebYarden.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\CANDLEhebYarden.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\HOThebYarden.wav</t>
-  </si>
-  <si>
-    <t>C:\Users\yarde\Documents\GitHub\BCI4ALS-MI\INDICATORhebYarden.wav</t>
-  </si>
-  <si>
     <t>target</t>
+  </si>
+  <si>
+    <t>YEShebYardenSHORT.wav</t>
+  </si>
+  <si>
+    <t>NOhebYardenSHORT.wav</t>
+  </si>
+  <si>
+    <t>PinkNoise.wav</t>
+  </si>
+  <si>
+    <t>CAMEhebYarden.wav</t>
+  </si>
+  <si>
+    <t>HOThebYarden.wav</t>
+  </si>
+  <si>
+    <t>INDICATORhebYarden.wav</t>
+  </si>
+  <si>
+    <t>CANDLEhebYarden.wav</t>
   </si>
 </sst>
 </file>
@@ -681,8 +681,8 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:E17"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -706,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -720,7 +720,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -737,7 +737,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -754,7 +754,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -762,16 +762,16 @@
     </row>
     <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
@@ -779,10 +779,10 @@
     </row>
     <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -796,10 +796,10 @@
     </row>
     <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -813,16 +813,16 @@
     </row>
     <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -839,7 +839,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
@@ -856,7 +856,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
@@ -864,16 +864,16 @@
     </row>
     <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2">
         <v>0</v>
@@ -881,16 +881,16 @@
     </row>
     <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E12" s="2">
         <v>0</v>
@@ -907,7 +907,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2">
         <v>1</v>
@@ -924,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
@@ -932,16 +932,16 @@
     </row>
     <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2">
         <v>0</v>
@@ -949,16 +949,16 @@
     </row>
     <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -966,10 +966,10 @@
     </row>
     <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -994,6 +994,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9F5CAB0486A994CA2C3B13E059EF2AE" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8645ec4a60d0c8c7009d2d6675847a91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="636d7205651659ec4fcda0bcbde9384b">
     <xsd:element name="properties">
@@ -1107,12 +1113,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1123,6 +1123,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFF1C174-6AC6-4774-A736-3226A12360E4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1138,21 +1153,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3725960-8A89-4E70-9C40-340E0EDB6403}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3744155D-8FAB-4E67-B5E0-C7FDBFB3715D}">
   <ds:schemaRefs>

</xml_diff>